<commit_message>
Update to pert table
</commit_message>
<xml_diff>
--- a/Table for PERT.xlsx
+++ b/Table for PERT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\ATHENAS-GLARE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73ACA0BE-16E2-48BB-9D6F-6254F14ED1AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DDABE1-6D80-4768-9641-9687992BF1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{DD965306-DB0E-46FB-89B3-7DB0EAF1B8B7}"/>
   </bookViews>
@@ -292,6 +292,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -302,9 +305,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -337,9 +337,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>22</xdr:col>
-          <xdr:colOff>96049</xdr:colOff>
+          <xdr:colOff>75224</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>7309</xdr:rowOff>
+          <xdr:rowOff>7310</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -354,7 +354,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$4:$H$6" spid="_x0000_s2032"/>
+                  <a14:cameraTool cellRange="$F$4:$H$6" spid="_x0000_s2095"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -368,8 +368,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="5321192" y="3229481"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="5309833" y="3154701"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -402,7 +402,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>96048</xdr:colOff>
+          <xdr:colOff>75223</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>8192</xdr:rowOff>
         </xdr:to>
@@ -419,7 +419,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$4:$L$6" spid="_x0000_s2033"/>
+                  <a14:cameraTool cellRange="$J$4:$L$6" spid="_x0000_s2096"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -433,8 +433,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="6845192" y="1314478"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="6900093" y="1300279"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -467,7 +467,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>96049</xdr:colOff>
+          <xdr:colOff>75224</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>8193</xdr:rowOff>
         </xdr:to>
@@ -484,7 +484,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$4:$P$6" spid="_x0000_s2034"/>
+                  <a14:cameraTool cellRange="$N$4:$P$6" spid="_x0000_s2097"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -498,8 +498,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="6888735" y="2272422"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="6900094" y="2227932"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -527,14 +527,14 @@
         <xdr:from>
           <xdr:col>25</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>235910</xdr:rowOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>87085</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>383</xdr:rowOff>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -549,7 +549,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$8:$D$10" spid="_x0000_s2035"/>
+                  <a14:cameraTool cellRange="$B$8:$D$10" spid="_x0000_s2098"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -563,8 +563,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="6662057" y="3218596"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="6891130" y="3151388"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -592,14 +592,14 @@
         <xdr:from>
           <xdr:col>25</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>14</xdr:row>
-          <xdr:rowOff>235909</xdr:rowOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>3996</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>87085</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>382</xdr:rowOff>
+          <xdr:rowOff>3995</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -614,7 +614,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$8:$H$10" spid="_x0000_s2036"/>
+                  <a14:cameraTool cellRange="$F$8:$H$10" spid="_x0000_s2099"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -628,8 +628,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="6749143" y="4176538"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="6891130" y="4079039"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -657,14 +657,14 @@
         <xdr:from>
           <xdr:col>25</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>235909</xdr:rowOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>3996</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>87085</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>381</xdr:rowOff>
+          <xdr:rowOff>3996</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -679,7 +679,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$8:$L$10" spid="_x0000_s2037"/>
+                  <a14:cameraTool cellRange="$J$8:$L$10" spid="_x0000_s2100"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -693,8 +693,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="6836229" y="5134480"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="6891130" y="5006692"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1002,14 +1002,14 @@
         <xdr:from>
           <xdr:col>31</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>235910</xdr:rowOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>34</xdr:col>
-          <xdr:colOff>87085</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>383</xdr:rowOff>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -1024,7 +1024,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$8:$P$10" spid="_x0000_s2038"/>
+                  <a14:cameraTool cellRange="$N$8:$P$10" spid="_x0000_s2101"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1038,8 +1038,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="8447314" y="3218596"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="8481391" y="3151388"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1067,14 +1067,14 @@
         <xdr:from>
           <xdr:col>31</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>235908</xdr:rowOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>3995</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>34</xdr:col>
-          <xdr:colOff>87085</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>381</xdr:rowOff>
+          <xdr:rowOff>3995</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -1089,7 +1089,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$12:$D$14" spid="_x0000_s2039"/>
+                  <a14:cameraTool cellRange="$B$12:$D$14" spid="_x0000_s2102"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1103,8 +1103,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="8229600" y="1302708"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="8481391" y="1296082"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1137,7 +1137,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>38</xdr:col>
-          <xdr:colOff>85601</xdr:colOff>
+          <xdr:colOff>60989</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>7310</xdr:rowOff>
         </xdr:to>
@@ -1154,7 +1154,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$12:$H$14" spid="_x0000_s2040"/>
+                  <a14:cameraTool cellRange="$F$12:$H$14" spid="_x0000_s2103"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1168,8 +1168,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="9490858" y="2271539"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="9536294" y="2227049"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1197,14 +1197,14 @@
         <xdr:from>
           <xdr:col>39</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>235910</xdr:rowOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>42</xdr:col>
-          <xdr:colOff>87085</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>383</xdr:rowOff>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -1219,7 +1219,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$12:$L$14" spid="_x0000_s2041"/>
+                  <a14:cameraTool cellRange="$J$12:$L$14" spid="_x0000_s2104"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1233,8 +1233,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="10493829" y="3218596"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="10601739" y="3151388"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1267,7 +1267,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>42</xdr:col>
-          <xdr:colOff>96048</xdr:colOff>
+          <xdr:colOff>75223</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>20759</xdr:rowOff>
         </xdr:to>
@@ -1284,7 +1284,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$16:$H$18" spid="_x0000_s2042"/>
+                  <a14:cameraTool cellRange="$F$16:$H$18" spid="_x0000_s2105"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1298,8 +1298,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="10415706" y="4679845"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="10610702" y="4559629"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1332,7 +1332,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>47</xdr:col>
-          <xdr:colOff>87085</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>19</xdr:row>
           <xdr:rowOff>217981</xdr:rowOff>
         </xdr:to>
@@ -1349,7 +1349,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$16:$D$18" spid="_x0000_s2043"/>
+                  <a14:cameraTool cellRange="$B$16:$D$18" spid="_x0000_s2106"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1363,8 +1363,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="11625943" y="4637581"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="11926957" y="4524938"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1392,14 +1392,14 @@
         <xdr:from>
           <xdr:col>44</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>235910</xdr:rowOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>47</xdr:col>
-          <xdr:colOff>87085</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>383</xdr:rowOff>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -1414,7 +1414,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$12:$P$14" spid="_x0000_s2044"/>
+                  <a14:cameraTool cellRange="$N$12:$P$14" spid="_x0000_s2107"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1428,8 +1428,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="11843657" y="3218596"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="11926957" y="3151388"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1457,14 +1457,14 @@
         <xdr:from>
           <xdr:col>49</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>235910</xdr:rowOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>52</xdr:col>
-          <xdr:colOff>87086</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>383</xdr:rowOff>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -1479,7 +1479,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$16:$L$18" spid="_x0000_s2045"/>
+                  <a14:cameraTool cellRange="$J$16:$L$18" spid="_x0000_s2108"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1493,8 +1493,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="13106400" y="3218596"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="13252174" y="3151388"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1522,14 +1522,14 @@
         <xdr:from>
           <xdr:col>54</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>235910</xdr:rowOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>57</xdr:col>
-          <xdr:colOff>87086</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>383</xdr:rowOff>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -1544,7 +1544,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$16:$P$18" spid="_x0000_s2046"/>
+                  <a14:cameraTool cellRange="$N$16:$P$18" spid="_x0000_s2109"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1558,8 +1558,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="14456229" y="3218596"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="14577391" y="3151388"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1587,14 +1587,14 @@
         <xdr:from>
           <xdr:col>59</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>235910</xdr:rowOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>62</xdr:col>
-          <xdr:colOff>87085</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>383</xdr:rowOff>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -1609,7 +1609,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$20:$D$22" spid="_x0000_s2047"/>
+                  <a14:cameraTool cellRange="$B$20:$D$22" spid="_x0000_s2110"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1623,8 +1623,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="15544800" y="3218596"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="15902609" y="3151388"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1652,14 +1652,14 @@
         <xdr:from>
           <xdr:col>64</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>235910</xdr:rowOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>67</xdr:col>
-          <xdr:colOff>87086</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>383</xdr:rowOff>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -1674,7 +1674,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$20:$H$22" spid="_x0000_s2048"/>
+                  <a14:cameraTool cellRange="$F$20:$H$22" spid="_x0000_s2111"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1688,8 +1688,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="16938171" y="3218596"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="17227826" y="3151388"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1717,14 +1717,14 @@
         <xdr:from>
           <xdr:col>69</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>235910</xdr:rowOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>72</xdr:col>
-          <xdr:colOff>87086</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>383</xdr:rowOff>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -1739,7 +1739,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$20:$L$22" spid="_x0000_s2049"/>
+                  <a14:cameraTool cellRange="$J$20:$L$22" spid="_x0000_s2112"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1753,8 +1753,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="18331543" y="3218596"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="18553043" y="3151388"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1782,14 +1782,14 @@
         <xdr:from>
           <xdr:col>75</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>235911</xdr:rowOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>3998</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>78</xdr:col>
-          <xdr:colOff>87086</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>382</xdr:rowOff>
+          <xdr:rowOff>3998</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -1804,7 +1804,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$20:$P$22" spid="_x0000_s2050"/>
+                  <a14:cameraTool cellRange="$N$20:$P$22" spid="_x0000_s2113"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1818,8 +1818,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="19942629" y="1781682"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="20143304" y="1759911"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1847,14 +1847,14 @@
         <xdr:from>
           <xdr:col>75</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>235909</xdr:rowOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>3996</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>78</xdr:col>
-          <xdr:colOff>87086</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>381</xdr:rowOff>
+          <xdr:rowOff>3996</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -1869,7 +1869,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$24:$D$26" spid="_x0000_s2051"/>
+                  <a14:cameraTool cellRange="$B$24:$D$26" spid="_x0000_s2114"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1883,8 +1883,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="19724914" y="2739623"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="20143304" y="2687561"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1912,14 +1912,14 @@
         <xdr:from>
           <xdr:col>75</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>235910</xdr:rowOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>78</xdr:col>
-          <xdr:colOff>87086</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>383</xdr:rowOff>
+          <xdr:rowOff>3996</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -1934,7 +1934,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$24:$H$26" spid="_x0000_s2052"/>
+                  <a14:cameraTool cellRange="$F$24:$H$26" spid="_x0000_s2115"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1948,8 +1948,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="19812000" y="3697567"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="20143304" y="3615214"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1977,14 +1977,14 @@
         <xdr:from>
           <xdr:col>75</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>16</xdr:row>
-          <xdr:rowOff>235910</xdr:rowOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>78</xdr:col>
-          <xdr:colOff>87086</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>383</xdr:rowOff>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -1999,7 +1999,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$24:$L$26" spid="_x0000_s2053"/>
+                  <a14:cameraTool cellRange="$J$24:$L$26" spid="_x0000_s2116"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2013,8 +2013,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="19899086" y="4655510"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="20143304" y="4542867"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2042,14 +2042,14 @@
         <xdr:from>
           <xdr:col>81</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>235910</xdr:rowOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>84</xdr:col>
-          <xdr:colOff>87085</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>383</xdr:rowOff>
+          <xdr:rowOff>3997</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -2064,7 +2064,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$24:$P$26" spid="_x0000_s2054"/>
+                  <a14:cameraTool cellRange="$N$24:$P$26" spid="_x0000_s2117"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2078,8 +2078,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="21510171" y="3218596"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="21733565" y="3151388"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3472,7 +3472,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$28:$D$30" spid="_x0000_s2055"/>
+                  <a14:cameraTool cellRange="$B$28:$D$30" spid="_x0000_s2118"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3537,7 +3537,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$28:$H$30" spid="_x0000_s2056"/>
+                  <a14:cameraTool cellRange="$F$28:$H$30" spid="_x0000_s2119"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3701,7 +3701,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>87085</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>44</xdr:row>
           <xdr:rowOff>8964</xdr:rowOff>
         </xdr:to>
@@ -3718,7 +3718,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$28:$P$30" spid="_x0000_s2057"/>
+                  <a14:cameraTool cellRange="$N$28:$P$30" spid="_x0000_s2120"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3732,8 +3732,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="6618514" y="10415707"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="6626087" y="10113747"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3766,9 +3766,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>32</xdr:col>
-          <xdr:colOff>87086</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>39</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>4703</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -3783,7 +3783,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$28:$L$30" spid="_x0000_s2058"/>
+                  <a14:cameraTool cellRange="$J$28:$L$30" spid="_x0000_s2121"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3797,8 +3797,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="7881257" y="9209314"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="7951304" y="8945217"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3831,9 +3831,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>87085</xdr:colOff>
-          <xdr:row>48</xdr:row>
-          <xdr:rowOff>231320</xdr:rowOff>
+          <xdr:colOff>66261</xdr:colOff>
+          <xdr:row>49</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -3848,7 +3848,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$32:$P$34" spid="_x0000_s2059"/>
+                  <a14:cameraTool cellRange="$N$32:$P$34" spid="_x0000_s2122"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3862,8 +3862,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="6618514" y="11604171"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="6626087" y="11264348"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3896,7 +3896,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>35</xdr:col>
-          <xdr:colOff>65314</xdr:colOff>
+          <xdr:colOff>40703</xdr:colOff>
           <xdr:row>44</xdr:row>
           <xdr:rowOff>19850</xdr:rowOff>
         </xdr:to>
@@ -3913,7 +3913,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$32:$D$34" spid="_x0000_s2060"/>
+                  <a14:cameraTool cellRange="$B$32:$D$34" spid="_x0000_s2123"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3927,8 +3927,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="8686800" y="10426593"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="8720877" y="10124633"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3961,7 +3961,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>37</xdr:col>
-          <xdr:colOff>96051</xdr:colOff>
+          <xdr:colOff>75226</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>224118</xdr:rowOff>
         </xdr:to>
@@ -3978,7 +3978,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$32:$H$34" spid="_x0000_s2061"/>
+                  <a14:cameraTool cellRange="$F$32:$H$34" spid="_x0000_s2124"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3992,8 +3992,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="9109422" y="9193947"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="9285487" y="8937422"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4026,9 +4026,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>42</xdr:col>
-          <xdr:colOff>87085</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>39</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>4703</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -4043,7 +4043,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$32:$L$34" spid="_x0000_s2062"/>
+                  <a14:cameraTool cellRange="$J$32:$L$34" spid="_x0000_s2125"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4057,8 +4057,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="10493829" y="9209314"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="10601739" y="8945217"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4091,9 +4091,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>47</xdr:col>
-          <xdr:colOff>97971</xdr:colOff>
+          <xdr:colOff>77147</xdr:colOff>
           <xdr:row>39</xdr:row>
-          <xdr:rowOff>21771</xdr:rowOff>
+          <xdr:rowOff>21770</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -4108,7 +4108,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$36:$D$38" spid="_x0000_s2063"/>
+                  <a14:cameraTool cellRange="$B$36:$D$38" spid="_x0000_s2126"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4122,8 +4122,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="11854543" y="9231085"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="11937843" y="8966988"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4156,7 +4156,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>47</xdr:col>
-          <xdr:colOff>96049</xdr:colOff>
+          <xdr:colOff>75225</xdr:colOff>
           <xdr:row>43</xdr:row>
           <xdr:rowOff>224118</xdr:rowOff>
         </xdr:to>
@@ -4173,7 +4173,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$36:$L$38" spid="_x0000_s2064"/>
+                  <a14:cameraTool cellRange="$J$36:$L$38" spid="_x0000_s2127"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4187,8 +4187,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="11809078" y="10391375"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="11935921" y="10096988"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4221,7 +4221,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>58</xdr:col>
-          <xdr:colOff>76199</xdr:colOff>
+          <xdr:colOff>51587</xdr:colOff>
           <xdr:row>34</xdr:row>
           <xdr:rowOff>228598</xdr:rowOff>
         </xdr:to>
@@ -4238,7 +4238,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$36:$H$38" spid="_x0000_s2065"/>
+                  <a14:cameraTool cellRange="$F$36:$H$38" spid="_x0000_s2128"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4252,8 +4252,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="14706599" y="8240484"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="14827761" y="8014250"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4286,7 +4286,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>47</xdr:col>
-          <xdr:colOff>95488</xdr:colOff>
+          <xdr:colOff>74664</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>8364</xdr:rowOff>
         </xdr:to>
@@ -4303,7 +4303,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$40:$H$42" spid="_x0000_s2066"/>
+                  <a14:cameraTool cellRange="$F$40:$H$42" spid="_x0000_s2129"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4317,8 +4317,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="11721432" y="7301793"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="11935360" y="7098277"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4351,7 +4351,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>52</xdr:col>
-          <xdr:colOff>87086</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>34</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4368,7 +4368,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$40:$L$42" spid="_x0000_s2067"/>
+                  <a14:cameraTool cellRange="$J$40:$L$42" spid="_x0000_s2130"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4382,8 +4382,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="13106400" y="8011886"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="13252174" y="7785652"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4416,7 +4416,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>55</xdr:col>
-          <xdr:colOff>113211</xdr:colOff>
+          <xdr:colOff>92386</xdr:colOff>
           <xdr:row>43</xdr:row>
           <xdr:rowOff>217715</xdr:rowOff>
         </xdr:to>
@@ -4433,7 +4433,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$36:$P$38" spid="_x0000_s2068"/>
+                  <a14:cameraTool cellRange="$N$36:$P$38" spid="_x0000_s2131"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4447,8 +4447,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="13959840" y="10384972"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="14073430" y="10090585"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4481,7 +4481,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>60</xdr:col>
-          <xdr:colOff>87086</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>44</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4498,7 +4498,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$40:$D$42" spid="_x0000_s2069"/>
+                  <a14:cameraTool cellRange="$B$40:$D$42" spid="_x0000_s2132"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4512,8 +4512,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="15022286" y="10406743"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="15372522" y="10104783"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4546,9 +4546,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>65</xdr:col>
-          <xdr:colOff>87086</xdr:colOff>
-          <xdr:row>48</xdr:row>
-          <xdr:rowOff>231320</xdr:rowOff>
+          <xdr:colOff>66260</xdr:colOff>
+          <xdr:row>49</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -4563,7 +4563,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$44:$P$46" spid="_x0000_s2070"/>
+                  <a14:cameraTool cellRange="$N$44:$P$46" spid="_x0000_s2133"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4577,8 +4577,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="16546286" y="11604171"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="16697739" y="11264348"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4611,7 +4611,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>55</xdr:col>
-          <xdr:colOff>87086</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4628,7 +4628,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$44:$D$46" spid="_x0000_s2071"/>
+                  <a14:cameraTool cellRange="$B$44:$D$46" spid="_x0000_s2134"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4642,8 +4642,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="13716001" y="7293429"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="14047305" y="7089913"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4676,7 +4676,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>60</xdr:col>
-          <xdr:colOff>97971</xdr:colOff>
+          <xdr:colOff>77146</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4693,7 +4693,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$44:$H$46" spid="_x0000_s2072"/>
+                  <a14:cameraTool cellRange="$F$44:$H$46" spid="_x0000_s2135"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4707,8 +4707,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="15120256" y="7293429"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="15383407" y="7089913"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4741,7 +4741,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>65</xdr:col>
-          <xdr:colOff>87086</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4758,7 +4758,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$44:$L$46" spid="_x0000_s2073"/>
+                  <a14:cameraTool cellRange="$J$44:$L$46" spid="_x0000_s2136"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4772,8 +4772,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="16502743" y="7293429"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="16697739" y="7089913"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4806,9 +4806,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>64</xdr:col>
-          <xdr:colOff>250371</xdr:colOff>
+          <xdr:colOff>229546</xdr:colOff>
           <xdr:row>39</xdr:row>
-          <xdr:rowOff>21771</xdr:rowOff>
+          <xdr:rowOff>21770</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -4823,7 +4823,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$48:$D$50" spid="_x0000_s2074"/>
+                  <a14:cameraTool cellRange="$B$48:$D$50" spid="_x0000_s2137"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4837,8 +4837,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="16448314" y="9231085"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="16595981" y="8966988"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4871,9 +4871,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>70</xdr:col>
-          <xdr:colOff>54429</xdr:colOff>
+          <xdr:colOff>29818</xdr:colOff>
           <xdr:row>39</xdr:row>
-          <xdr:rowOff>21771</xdr:rowOff>
+          <xdr:rowOff>21770</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -4888,7 +4888,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$48:$H$50" spid="_x0000_s2075"/>
+                  <a14:cameraTool cellRange="$F$48:$H$50" spid="_x0000_s2138"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4902,8 +4902,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="17819915" y="9231085"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="17986514" y="8966988"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4936,7 +4936,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>75</xdr:col>
-          <xdr:colOff>130626</xdr:colOff>
+          <xdr:colOff>109802</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>217713</xdr:rowOff>
         </xdr:to>
@@ -4953,7 +4953,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$48:$L$50" spid="_x0000_s2076"/>
+                  <a14:cameraTool cellRange="$J$48:$L$50" spid="_x0000_s2139"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4967,8 +4967,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="19202398" y="9187542"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="19391715" y="8931017"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5001,7 +5001,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>80</xdr:col>
-          <xdr:colOff>108857</xdr:colOff>
+          <xdr:colOff>88031</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>228599</xdr:rowOff>
         </xdr:to>
@@ -5018,7 +5018,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$48:$P$50" spid="_x0000_s2077"/>
+                  <a14:cameraTool cellRange="$N$48:$P$50" spid="_x0000_s2140"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -5032,8 +5032,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="20486914" y="9198428"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="20695162" y="8941903"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5083,7 +5083,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$52:$H$54" spid="_x0000_s2078"/>
+                  <a14:cameraTool cellRange="$F$52:$H$54" spid="_x0000_s2141"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -5148,7 +5148,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$52:$L$54" spid="_x0000_s2079"/>
+                  <a14:cameraTool cellRange="$J$52:$L$54" spid="_x0000_s2142"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -5196,9 +5196,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>36</xdr:col>
-          <xdr:colOff>105048</xdr:colOff>
+          <xdr:colOff>82044</xdr:colOff>
           <xdr:row>64</xdr:row>
-          <xdr:rowOff>112666</xdr:rowOff>
+          <xdr:rowOff>112665</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -5213,7 +5213,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$52:$P$54" spid="_x0000_s2080"/>
+                  <a14:cameraTool cellRange="$N$52:$P$54" spid="_x0000_s2143"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -5227,8 +5227,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="8985613" y="15309123"/>
-              <a:ext cx="873035" cy="718457"/>
+              <a:off x="9027262" y="14855709"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6736,7 +6736,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$52:$D$54" spid="_x0000_s2081"/>
+                  <a14:cameraTool cellRange="$B$52:$D$54" spid="_x0000_s2144"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -6952,9 +6952,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>53</xdr:col>
-          <xdr:colOff>97971</xdr:colOff>
+          <xdr:colOff>77145</xdr:colOff>
           <xdr:row>40</xdr:row>
-          <xdr:rowOff>21771</xdr:rowOff>
+          <xdr:rowOff>21770</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -6969,7 +6969,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$40:$P$42" spid="_x0000_s2082"/>
+                  <a14:cameraTool cellRange="$N$40:$P$42" spid="_x0000_s2145"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -6983,8 +6983,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="13422085" y="9470571"/>
-              <a:ext cx="870857" cy="718457"/>
+              <a:off x="13528102" y="9198901"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7189,9 +7189,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>41</xdr:col>
-          <xdr:colOff>83127</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>64</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>723</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -7206,7 +7206,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$56:$D$58" spid="_x0000_s2083"/>
+                  <a14:cameraTool cellRange="$B$56:$D$58" spid="_x0000_s2146"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7220,8 +7220,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="10335491" y="14962909"/>
-              <a:ext cx="872836" cy="706582"/>
+              <a:off x="10336696" y="14743043"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7254,9 +7254,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>46</xdr:col>
-          <xdr:colOff>83127</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>64</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>723</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -7271,7 +7271,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$56:$H$58" spid="_x0000_s2084"/>
+                  <a14:cameraTool cellRange="$F$56:$H$58" spid="_x0000_s2147"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7285,8 +7285,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="11651673" y="14962909"/>
-              <a:ext cx="872836" cy="706582"/>
+              <a:off x="11661913" y="14743043"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7319,9 +7319,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>51</xdr:col>
-          <xdr:colOff>83127</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>64</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>723</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -7336,7 +7336,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$56:$L$58" spid="_x0000_s2085"/>
+                  <a14:cameraTool cellRange="$J$56:$L$58" spid="_x0000_s2148"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7350,8 +7350,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="12967855" y="14962909"/>
-              <a:ext cx="872836" cy="706582"/>
+              <a:off x="12987130" y="14743043"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7384,9 +7384,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>56</xdr:col>
-          <xdr:colOff>83127</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>64</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>723</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -7401,7 +7401,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$56:$P$58" spid="_x0000_s2086"/>
+                  <a14:cameraTool cellRange="$N$56:$P$58" spid="_x0000_s2149"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7415,8 +7415,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="14284036" y="14962909"/>
-              <a:ext cx="872836" cy="706582"/>
+              <a:off x="14312348" y="14743043"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7449,9 +7449,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>61</xdr:col>
-          <xdr:colOff>83127</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>64</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>723</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -7466,7 +7466,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$60:$D$62" spid="_x0000_s2087"/>
+                  <a14:cameraTool cellRange="$B$60:$D$62" spid="_x0000_s2150"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7480,8 +7480,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="15600218" y="14962909"/>
-              <a:ext cx="872836" cy="706582"/>
+              <a:off x="15637565" y="14743043"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7514,7 +7514,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>64</xdr:col>
-          <xdr:colOff>70263</xdr:colOff>
+          <xdr:colOff>51589</xdr:colOff>
           <xdr:row>59</xdr:row>
           <xdr:rowOff>10885</xdr:rowOff>
         </xdr:to>
@@ -7531,7 +7531,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$60:$H$62" spid="_x0000_s2088"/>
+                  <a14:cameraTool cellRange="$F$60:$H$62" spid="_x0000_s2151"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7545,8 +7545,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="16377063" y="13796158"/>
-              <a:ext cx="872836" cy="706582"/>
+              <a:off x="16418024" y="13594363"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7579,7 +7579,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>64</xdr:col>
-          <xdr:colOff>83127</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>69</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -7596,7 +7596,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$60:$L$62" spid="_x0000_s2089"/>
+                  <a14:cameraTool cellRange="$J$60:$L$62" spid="_x0000_s2152"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7610,8 +7610,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="16389927" y="16140545"/>
-              <a:ext cx="872836" cy="706582"/>
+              <a:off x="16432696" y="15902609"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7644,9 +7644,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>70</xdr:col>
-          <xdr:colOff>83126</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>64</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>723</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -7661,7 +7661,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$60:$P$62" spid="_x0000_s2090"/>
+                  <a14:cameraTool cellRange="$N$60:$P$62" spid="_x0000_s2153"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7675,8 +7675,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="17969345" y="14962909"/>
-              <a:ext cx="872836" cy="706582"/>
+              <a:off x="18022957" y="14743043"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7709,7 +7709,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>70</xdr:col>
-          <xdr:colOff>83126</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>69</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -7726,7 +7726,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$64:$D$66" spid="_x0000_s2091"/>
+                  <a14:cameraTool cellRange="$B$64:$D$66" spid="_x0000_s2154"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7740,8 +7740,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="17969345" y="16140545"/>
-              <a:ext cx="872836" cy="706582"/>
+              <a:off x="18022957" y="15902609"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7774,7 +7774,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>70</xdr:col>
-          <xdr:colOff>83126</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>74</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -7791,7 +7791,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$F$64:$H$66" spid="_x0000_s2092"/>
+                  <a14:cameraTool cellRange="$F$64:$H$66" spid="_x0000_s2155"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7805,8 +7805,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="17969345" y="17318182"/>
-              <a:ext cx="872836" cy="706582"/>
+              <a:off x="18022957" y="17062174"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7839,7 +7839,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>75</xdr:col>
-          <xdr:colOff>83127</xdr:colOff>
+          <xdr:colOff>66261</xdr:colOff>
           <xdr:row>69</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -7856,7 +7856,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$J$64:$L$66" spid="_x0000_s2093"/>
+                  <a14:cameraTool cellRange="$J$64:$L$66" spid="_x0000_s2156"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7870,8 +7870,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="19285527" y="16140545"/>
-              <a:ext cx="872836" cy="706582"/>
+              <a:off x="19348174" y="15902609"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7904,7 +7904,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>80</xdr:col>
-          <xdr:colOff>83127</xdr:colOff>
+          <xdr:colOff>66260</xdr:colOff>
           <xdr:row>69</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -7921,7 +7921,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$N$64:$P$66" spid="_x0000_s2094"/>
+                  <a14:cameraTool cellRange="$N$64:$P$66" spid="_x0000_s2157"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7935,8 +7935,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="20601709" y="16140545"/>
-              <a:ext cx="872836" cy="706582"/>
+              <a:off x="20673391" y="15902609"/>
+              <a:ext cx="861391" cy="695739"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -9044,7 +9044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96151AB6-C34B-4110-B17F-9E53EBB39427}">
   <dimension ref="A1:CK66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="46" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="17" topLeftCell="R1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AA55" sqref="AA55"/>
     </sheetView>
@@ -9086,23 +9086,23 @@
     </row>
     <row r="2" spans="1:17" s="2" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
       <c r="Q2" s="9"/>
     </row>
     <row r="4" spans="1:17" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -9144,26 +9144,26 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
-      <c r="F5" s="15">
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
+      <c r="F5" s="16">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="17"/>
-      <c r="J5" s="15">
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
+      <c r="J5" s="16">
         <v>1.2</v>
       </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="17"/>
-      <c r="N5" s="15">
+      <c r="K5" s="17"/>
+      <c r="L5" s="18"/>
+      <c r="N5" s="16">
         <v>1.3</v>
       </c>
-      <c r="O5" s="16"/>
-      <c r="P5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="18"/>
     </row>
     <row r="6" spans="1:17" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
@@ -9178,7 +9178,7 @@
       <c r="F6" s="3">
         <v>16</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="15">
         <v>16</v>
       </c>
       <c r="H6" s="3">
@@ -9187,7 +9187,7 @@
       <c r="J6" s="3">
         <v>17</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="15">
         <v>16</v>
       </c>
       <c r="L6" s="3">
@@ -9196,7 +9196,7 @@
       <c r="N6" s="3">
         <v>17</v>
       </c>
-      <c r="O6" s="19">
+      <c r="O6" s="15">
         <v>16</v>
       </c>
       <c r="P6" s="3">
@@ -9242,32 +9242,32 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="15">
+      <c r="B9" s="16">
         <v>1.4</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
-      <c r="F9" s="15">
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="F9" s="16">
         <v>1.5</v>
       </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="17"/>
-      <c r="J9" s="15">
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+      <c r="J9" s="16">
         <v>1.6</v>
       </c>
-      <c r="K9" s="16"/>
-      <c r="L9" s="17"/>
-      <c r="N9" s="15">
+      <c r="K9" s="17"/>
+      <c r="L9" s="18"/>
+      <c r="N9" s="16">
         <v>1.7</v>
       </c>
-      <c r="O9" s="16"/>
-      <c r="P9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="18"/>
     </row>
     <row r="10" spans="1:17" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>17</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="15">
         <v>16</v>
       </c>
       <c r="D10" s="3">
@@ -9276,7 +9276,7 @@
       <c r="F10" s="3">
         <v>17</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="15">
         <v>16</v>
       </c>
       <c r="H10" s="3">
@@ -9285,7 +9285,7 @@
       <c r="J10" s="3">
         <v>17</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="15">
         <v>16</v>
       </c>
       <c r="L10" s="3">
@@ -9340,32 +9340,32 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="15">
+      <c r="B13" s="16">
         <v>1.8</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="17"/>
-      <c r="F13" s="15">
+      <c r="C13" s="17"/>
+      <c r="D13" s="18"/>
+      <c r="F13" s="16">
         <v>1.9</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="17"/>
-      <c r="J13" s="15" t="s">
+      <c r="G13" s="17"/>
+      <c r="H13" s="18"/>
+      <c r="J13" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K13" s="16"/>
-      <c r="L13" s="17"/>
-      <c r="N13" s="15">
+      <c r="K13" s="17"/>
+      <c r="L13" s="18"/>
+      <c r="N13" s="16">
         <v>1.1100000000000001</v>
       </c>
-      <c r="O13" s="16"/>
-      <c r="P13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="18"/>
     </row>
     <row r="14" spans="1:17" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>17</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="15">
         <v>17</v>
       </c>
       <c r="D14" s="3">
@@ -9374,7 +9374,7 @@
       <c r="F14" s="3">
         <v>25</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="15">
         <v>17</v>
       </c>
       <c r="H14" s="3">
@@ -9383,7 +9383,7 @@
       <c r="J14" s="3">
         <v>26</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="15">
         <v>16</v>
       </c>
       <c r="L14" s="3">
@@ -9392,7 +9392,7 @@
       <c r="N14" s="3">
         <v>27</v>
       </c>
-      <c r="O14" s="19">
+      <c r="O14" s="15">
         <v>16</v>
       </c>
       <c r="P14" s="3">
@@ -9438,32 +9438,32 @@
       </c>
     </row>
     <row r="17" spans="2:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="15">
+      <c r="B17" s="16">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-      <c r="F17" s="15">
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="F17" s="16">
         <v>2.1</v>
       </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="17"/>
-      <c r="J17" s="15">
+      <c r="G17" s="17"/>
+      <c r="H17" s="18"/>
+      <c r="J17" s="16">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K17" s="16"/>
-      <c r="L17" s="17"/>
-      <c r="N17" s="15">
+      <c r="K17" s="17"/>
+      <c r="L17" s="18"/>
+      <c r="N17" s="16">
         <v>2.2999999999999998</v>
       </c>
-      <c r="O17" s="16"/>
-      <c r="P17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="18"/>
     </row>
     <row r="18" spans="2:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <v>25</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="15">
         <v>15</v>
       </c>
       <c r="D18" s="3">
@@ -9472,7 +9472,7 @@
       <c r="F18" s="3">
         <v>23</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="15">
         <v>13</v>
       </c>
       <c r="H18" s="3">
@@ -9481,7 +9481,7 @@
       <c r="J18" s="3">
         <v>28</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="15">
         <v>16</v>
       </c>
       <c r="L18" s="3">
@@ -9490,7 +9490,7 @@
       <c r="N18" s="3">
         <v>29</v>
       </c>
-      <c r="O18" s="19">
+      <c r="O18" s="15">
         <v>16</v>
       </c>
       <c r="P18" s="3">
@@ -9541,32 +9541,32 @@
       </c>
     </row>
     <row r="21" spans="2:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="15">
+      <c r="B21" s="16">
         <v>2.4</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="17"/>
-      <c r="F21" s="15">
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
+      <c r="F21" s="16">
         <v>2.5</v>
       </c>
-      <c r="G21" s="16"/>
-      <c r="H21" s="17"/>
-      <c r="J21" s="15">
+      <c r="G21" s="17"/>
+      <c r="H21" s="18"/>
+      <c r="J21" s="16">
         <v>2.6</v>
       </c>
-      <c r="K21" s="16"/>
-      <c r="L21" s="17"/>
-      <c r="N21" s="15">
+      <c r="K21" s="17"/>
+      <c r="L21" s="18"/>
+      <c r="N21" s="16">
         <v>2.7</v>
       </c>
-      <c r="O21" s="16"/>
-      <c r="P21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="18"/>
     </row>
     <row r="22" spans="2:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <v>30</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="15">
         <v>16</v>
       </c>
       <c r="D22" s="3">
@@ -9575,7 +9575,7 @@
       <c r="F22" s="3">
         <v>31</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="15">
         <v>16</v>
       </c>
       <c r="H22" s="3">
@@ -9584,7 +9584,7 @@
       <c r="J22" s="3">
         <v>32</v>
       </c>
-      <c r="K22" s="19">
+      <c r="K22" s="15">
         <v>16</v>
       </c>
       <c r="L22" s="3">
@@ -9593,7 +9593,7 @@
       <c r="N22" s="3">
         <v>33</v>
       </c>
-      <c r="O22" s="19">
+      <c r="O22" s="15">
         <v>16</v>
       </c>
       <c r="P22" s="3">
@@ -9642,32 +9642,32 @@
       </c>
     </row>
     <row r="25" spans="2:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="15">
+      <c r="B25" s="16">
         <v>2.8</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="17"/>
-      <c r="F25" s="15">
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
+      <c r="F25" s="16">
         <v>2.9</v>
       </c>
-      <c r="G25" s="16"/>
-      <c r="H25" s="17"/>
-      <c r="J25" s="15" t="s">
+      <c r="G25" s="17"/>
+      <c r="H25" s="18"/>
+      <c r="J25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="K25" s="16"/>
-      <c r="L25" s="17"/>
-      <c r="N25" s="15">
+      <c r="K25" s="17"/>
+      <c r="L25" s="18"/>
+      <c r="N25" s="16">
         <v>2.11</v>
       </c>
-      <c r="O25" s="16"/>
-      <c r="P25" s="17"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="18"/>
     </row>
     <row r="26" spans="2:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <v>33</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="15">
         <v>16</v>
       </c>
       <c r="D26" s="3">
@@ -9676,7 +9676,7 @@
       <c r="F26" s="3">
         <v>33</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="15">
         <v>16</v>
       </c>
       <c r="H26" s="3">
@@ -9685,7 +9685,7 @@
       <c r="J26" s="3">
         <v>33</v>
       </c>
-      <c r="K26" s="19">
+      <c r="K26" s="15">
         <v>16</v>
       </c>
       <c r="L26" s="3">
@@ -9694,7 +9694,7 @@
       <c r="N26" s="3">
         <v>34</v>
       </c>
-      <c r="O26" s="19">
+      <c r="O26" s="15">
         <v>16</v>
       </c>
       <c r="P26" s="3">
@@ -9745,26 +9745,26 @@
       </c>
     </row>
     <row r="29" spans="2:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="15">
+      <c r="B29" s="16">
         <v>2.12</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="F29" s="15">
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="F29" s="16">
         <v>2.13</v>
       </c>
-      <c r="G29" s="16"/>
-      <c r="H29" s="17"/>
-      <c r="J29" s="15">
+      <c r="G29" s="17"/>
+      <c r="H29" s="18"/>
+      <c r="J29" s="16">
         <v>3.1</v>
       </c>
-      <c r="K29" s="16"/>
-      <c r="L29" s="17"/>
-      <c r="N29" s="15">
+      <c r="K29" s="17"/>
+      <c r="L29" s="18"/>
+      <c r="N29" s="16">
         <v>3.2</v>
       </c>
-      <c r="O29" s="16"/>
-      <c r="P29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="18"/>
       <c r="BJ29" t="s">
         <v>14</v>
       </c>
@@ -9773,7 +9773,7 @@
       <c r="B30" s="3">
         <v>35</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="15">
         <v>16</v>
       </c>
       <c r="D30" s="3">
@@ -9782,7 +9782,7 @@
       <c r="F30" s="3">
         <v>36</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="15">
         <v>16</v>
       </c>
       <c r="H30" s="3">
@@ -9791,7 +9791,7 @@
       <c r="J30" s="3">
         <v>37</v>
       </c>
-      <c r="K30" s="19">
+      <c r="K30" s="15">
         <v>16</v>
       </c>
       <c r="L30" s="3">
@@ -9800,7 +9800,7 @@
       <c r="N30" s="3">
         <v>29</v>
       </c>
-      <c r="O30" s="19">
+      <c r="O30" s="15">
         <v>8</v>
       </c>
       <c r="P30" s="3">
@@ -9849,32 +9849,32 @@
       </c>
     </row>
     <row r="33" spans="2:89" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="15">
+      <c r="B33" s="16">
         <v>3.3</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="17"/>
-      <c r="F33" s="15">
+      <c r="C33" s="17"/>
+      <c r="D33" s="18"/>
+      <c r="F33" s="16">
         <v>3.4</v>
       </c>
-      <c r="G33" s="16"/>
-      <c r="H33" s="17"/>
-      <c r="J33" s="15">
+      <c r="G33" s="17"/>
+      <c r="H33" s="18"/>
+      <c r="J33" s="16">
         <v>3.5</v>
       </c>
-      <c r="K33" s="16"/>
-      <c r="L33" s="17"/>
-      <c r="N33" s="15">
+      <c r="K33" s="17"/>
+      <c r="L33" s="18"/>
+      <c r="N33" s="16">
         <v>3.6</v>
       </c>
-      <c r="O33" s="16"/>
-      <c r="P33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="18"/>
     </row>
     <row r="34" spans="2:89" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="3">
         <v>37</v>
       </c>
-      <c r="C34" s="19">
+      <c r="C34" s="15">
         <v>9</v>
       </c>
       <c r="D34" s="3">
@@ -9883,7 +9883,7 @@
       <c r="F34" s="3">
         <v>38</v>
       </c>
-      <c r="G34" s="19">
+      <c r="G34" s="15">
         <v>9</v>
       </c>
       <c r="H34" s="3">
@@ -9892,7 +9892,7 @@
       <c r="J34" s="3">
         <v>45</v>
       </c>
-      <c r="K34" s="19">
+      <c r="K34" s="15">
         <v>9</v>
       </c>
       <c r="L34" s="3">
@@ -9901,7 +9901,7 @@
       <c r="N34" s="3">
         <v>28</v>
       </c>
-      <c r="O34" s="19">
+      <c r="O34" s="15">
         <v>0</v>
       </c>
       <c r="P34" s="3">
@@ -9955,26 +9955,26 @@
       </c>
     </row>
     <row r="37" spans="2:89" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="15">
+      <c r="B37" s="16">
         <v>3.7</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="17"/>
-      <c r="F37" s="15">
+      <c r="C37" s="17"/>
+      <c r="D37" s="18"/>
+      <c r="F37" s="16">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G37" s="16"/>
-      <c r="H37" s="17"/>
-      <c r="J37" s="15">
+      <c r="G37" s="17"/>
+      <c r="H37" s="18"/>
+      <c r="J37" s="16">
         <v>4.2</v>
       </c>
-      <c r="K37" s="16"/>
-      <c r="L37" s="17"/>
-      <c r="N37" s="15">
+      <c r="K37" s="17"/>
+      <c r="L37" s="18"/>
+      <c r="N37" s="16">
         <v>4.3</v>
       </c>
-      <c r="O37" s="16"/>
-      <c r="P37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="18"/>
       <c r="BF37" t="s">
         <v>15</v>
       </c>
@@ -9986,7 +9986,7 @@
       <c r="B38" s="3">
         <v>48</v>
       </c>
-      <c r="C38" s="19">
+      <c r="C38" s="15">
         <v>9</v>
       </c>
       <c r="D38" s="3">
@@ -9995,7 +9995,7 @@
       <c r="F38" s="3">
         <v>135</v>
       </c>
-      <c r="G38" s="19">
+      <c r="G38" s="15">
         <v>93</v>
       </c>
       <c r="H38" s="3">
@@ -10004,7 +10004,7 @@
       <c r="J38" s="3">
         <v>135</v>
       </c>
-      <c r="K38" s="19">
+      <c r="K38" s="15">
         <v>93</v>
       </c>
       <c r="L38" s="3">
@@ -10013,7 +10013,7 @@
       <c r="N38" s="3">
         <v>59</v>
       </c>
-      <c r="O38" s="19">
+      <c r="O38" s="15">
         <v>8</v>
       </c>
       <c r="P38" s="3">
@@ -10070,32 +10070,32 @@
       </c>
     </row>
     <row r="41" spans="2:89" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="15">
+      <c r="B41" s="16">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="17"/>
-      <c r="F41" s="15">
+      <c r="C41" s="17"/>
+      <c r="D41" s="18"/>
+      <c r="F41" s="16">
         <v>4.5</v>
       </c>
-      <c r="G41" s="16"/>
-      <c r="H41" s="17"/>
-      <c r="J41" s="15">
+      <c r="G41" s="17"/>
+      <c r="H41" s="18"/>
+      <c r="J41" s="16">
         <v>4.5999999999999996</v>
       </c>
-      <c r="K41" s="16"/>
-      <c r="L41" s="17"/>
-      <c r="N41" s="15">
+      <c r="K41" s="17"/>
+      <c r="L41" s="18"/>
+      <c r="N41" s="16">
         <v>4.7</v>
       </c>
-      <c r="O41" s="16"/>
-      <c r="P41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="18"/>
     </row>
     <row r="42" spans="2:89" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="3">
         <v>135</v>
       </c>
-      <c r="C42" s="19">
+      <c r="C42" s="15">
         <v>83</v>
       </c>
       <c r="D42" s="3">
@@ -10104,7 +10104,7 @@
       <c r="F42" s="3">
         <v>51</v>
       </c>
-      <c r="G42" s="19">
+      <c r="G42" s="15">
         <v>9</v>
       </c>
       <c r="H42" s="3">
@@ -10113,7 +10113,7 @@
       <c r="J42" s="3">
         <v>51</v>
       </c>
-      <c r="K42" s="19">
+      <c r="K42" s="15">
         <v>9</v>
       </c>
       <c r="L42" s="3">
@@ -10122,7 +10122,7 @@
       <c r="N42" s="3">
         <v>51</v>
       </c>
-      <c r="O42" s="19">
+      <c r="O42" s="15">
         <v>9</v>
       </c>
       <c r="P42" s="3">
@@ -10171,32 +10171,32 @@
       </c>
     </row>
     <row r="45" spans="2:89" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="15">
+      <c r="B45" s="16">
         <v>4.8</v>
       </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="17"/>
-      <c r="F45" s="15">
+      <c r="C45" s="17"/>
+      <c r="D45" s="18"/>
+      <c r="F45" s="16">
         <v>4.9000000000000004</v>
       </c>
-      <c r="G45" s="16"/>
-      <c r="H45" s="17"/>
-      <c r="J45" s="15" t="s">
+      <c r="G45" s="17"/>
+      <c r="H45" s="18"/>
+      <c r="J45" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="K45" s="16"/>
-      <c r="L45" s="17"/>
-      <c r="N45" s="15">
+      <c r="K45" s="17"/>
+      <c r="L45" s="18"/>
+      <c r="N45" s="16">
         <v>4.1100000000000003</v>
       </c>
-      <c r="O45" s="16"/>
-      <c r="P45" s="17"/>
+      <c r="O45" s="17"/>
+      <c r="P45" s="18"/>
     </row>
     <row r="46" spans="2:89" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="3">
         <v>60</v>
       </c>
-      <c r="C46" s="19">
+      <c r="C46" s="15">
         <v>8</v>
       </c>
       <c r="D46" s="3">
@@ -10205,7 +10205,7 @@
       <c r="F46" s="3">
         <v>69</v>
       </c>
-      <c r="G46" s="19">
+      <c r="G46" s="15">
         <v>8</v>
       </c>
       <c r="H46" s="3">
@@ -10214,7 +10214,7 @@
       <c r="J46" s="3">
         <v>78</v>
       </c>
-      <c r="K46" s="19">
+      <c r="K46" s="15">
         <v>8</v>
       </c>
       <c r="L46" s="3">
@@ -10223,7 +10223,7 @@
       <c r="N46" s="3">
         <v>78</v>
       </c>
-      <c r="O46" s="19">
+      <c r="O46" s="15">
         <v>36</v>
       </c>
       <c r="P46" s="3">
@@ -10269,32 +10269,32 @@
       </c>
     </row>
     <row r="49" spans="2:54" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="15">
+      <c r="B49" s="16">
         <v>4.12</v>
       </c>
-      <c r="C49" s="16"/>
-      <c r="D49" s="17"/>
-      <c r="F49" s="15">
+      <c r="C49" s="17"/>
+      <c r="D49" s="18"/>
+      <c r="F49" s="16">
         <v>4.13</v>
       </c>
-      <c r="G49" s="16"/>
-      <c r="H49" s="17"/>
-      <c r="J49" s="15">
+      <c r="G49" s="17"/>
+      <c r="H49" s="18"/>
+      <c r="J49" s="16">
         <v>4.1399999999999997</v>
       </c>
-      <c r="K49" s="16"/>
-      <c r="L49" s="17"/>
-      <c r="N49" s="15">
+      <c r="K49" s="17"/>
+      <c r="L49" s="18"/>
+      <c r="N49" s="16">
         <v>4.1500000000000004</v>
       </c>
-      <c r="O49" s="16"/>
-      <c r="P49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="18"/>
     </row>
     <row r="50" spans="2:54" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="3">
         <v>87</v>
       </c>
-      <c r="C50" s="19">
+      <c r="C50" s="15">
         <v>8</v>
       </c>
       <c r="D50" s="3">
@@ -10303,7 +10303,7 @@
       <c r="F50" s="3">
         <v>88</v>
       </c>
-      <c r="G50" s="19">
+      <c r="G50" s="15">
         <v>8</v>
       </c>
       <c r="H50" s="3">
@@ -10312,7 +10312,7 @@
       <c r="J50" s="3">
         <v>97</v>
       </c>
-      <c r="K50" s="19">
+      <c r="K50" s="15">
         <v>8</v>
       </c>
       <c r="L50" s="3">
@@ -10321,7 +10321,7 @@
       <c r="N50" s="3">
         <v>106</v>
       </c>
-      <c r="O50" s="19">
+      <c r="O50" s="15">
         <v>8</v>
       </c>
       <c r="P50" s="3">
@@ -10370,32 +10370,32 @@
       </c>
     </row>
     <row r="53" spans="2:54" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="15">
+      <c r="B53" s="16">
         <v>4.16</v>
       </c>
-      <c r="C53" s="16"/>
-      <c r="D53" s="17"/>
-      <c r="F53" s="15">
+      <c r="C53" s="17"/>
+      <c r="D53" s="18"/>
+      <c r="F53" s="16">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G53" s="16"/>
-      <c r="H53" s="17"/>
-      <c r="J53" s="15">
+      <c r="G53" s="17"/>
+      <c r="H53" s="18"/>
+      <c r="J53" s="16">
         <v>5.2</v>
       </c>
-      <c r="K53" s="16"/>
-      <c r="L53" s="17"/>
-      <c r="N53" s="15">
+      <c r="K53" s="17"/>
+      <c r="L53" s="18"/>
+      <c r="N53" s="16">
         <v>5.3</v>
       </c>
-      <c r="O53" s="16"/>
-      <c r="P53" s="17"/>
+      <c r="O53" s="17"/>
+      <c r="P53" s="18"/>
     </row>
     <row r="54" spans="2:54" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="3">
         <v>115</v>
       </c>
-      <c r="C54" s="19">
+      <c r="C54" s="15">
         <v>8</v>
       </c>
       <c r="D54" s="3">
@@ -10413,7 +10413,7 @@
       <c r="J54" s="3">
         <v>118</v>
       </c>
-      <c r="K54" s="19">
+      <c r="K54" s="15">
         <v>8</v>
       </c>
       <c r="L54" s="3">
@@ -10422,7 +10422,7 @@
       <c r="N54" s="3">
         <v>119</v>
       </c>
-      <c r="O54" s="19">
+      <c r="O54" s="15">
         <v>8</v>
       </c>
       <c r="P54" s="3">
@@ -10468,32 +10468,32 @@
       </c>
     </row>
     <row r="57" spans="2:54" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="15">
+      <c r="B57" s="16">
         <v>5.4</v>
       </c>
-      <c r="C57" s="16"/>
-      <c r="D57" s="17"/>
-      <c r="F57" s="15">
+      <c r="C57" s="17"/>
+      <c r="D57" s="18"/>
+      <c r="F57" s="16">
         <v>5.5</v>
       </c>
-      <c r="G57" s="16"/>
-      <c r="H57" s="17"/>
-      <c r="J57" s="15">
+      <c r="G57" s="17"/>
+      <c r="H57" s="18"/>
+      <c r="J57" s="16">
         <v>5.6</v>
       </c>
-      <c r="K57" s="16"/>
-      <c r="L57" s="17"/>
-      <c r="N57" s="15">
+      <c r="K57" s="17"/>
+      <c r="L57" s="18"/>
+      <c r="N57" s="16">
         <v>5.7</v>
       </c>
-      <c r="O57" s="16"/>
-      <c r="P57" s="17"/>
+      <c r="O57" s="17"/>
+      <c r="P57" s="18"/>
     </row>
     <row r="58" spans="2:54" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="3">
         <v>122</v>
       </c>
-      <c r="C58" s="19">
+      <c r="C58" s="15">
         <v>8</v>
       </c>
       <c r="D58" s="3">
@@ -10502,7 +10502,7 @@
       <c r="F58" s="3">
         <v>125</v>
       </c>
-      <c r="G58" s="19">
+      <c r="G58" s="15">
         <v>8</v>
       </c>
       <c r="H58" s="3">
@@ -10511,7 +10511,7 @@
       <c r="J58" s="3">
         <v>126</v>
       </c>
-      <c r="K58" s="19">
+      <c r="K58" s="15">
         <v>8</v>
       </c>
       <c r="L58" s="3">
@@ -10520,7 +10520,7 @@
       <c r="N58" s="3">
         <v>129</v>
       </c>
-      <c r="O58" s="19">
+      <c r="O58" s="15">
         <v>8</v>
       </c>
       <c r="P58" s="3">
@@ -10566,32 +10566,32 @@
       </c>
     </row>
     <row r="61" spans="2:54" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="15">
+      <c r="B61" s="16">
         <v>5.8</v>
       </c>
-      <c r="C61" s="16"/>
-      <c r="D61" s="17"/>
-      <c r="F61" s="15">
+      <c r="C61" s="17"/>
+      <c r="D61" s="18"/>
+      <c r="F61" s="16">
         <v>6.1</v>
       </c>
-      <c r="G61" s="16"/>
-      <c r="H61" s="17"/>
-      <c r="J61" s="15">
+      <c r="G61" s="17"/>
+      <c r="H61" s="18"/>
+      <c r="J61" s="16">
         <v>6.2</v>
       </c>
-      <c r="K61" s="16"/>
-      <c r="L61" s="17"/>
-      <c r="N61" s="15">
+      <c r="K61" s="17"/>
+      <c r="L61" s="18"/>
+      <c r="N61" s="16">
         <v>6.3</v>
       </c>
-      <c r="O61" s="16"/>
-      <c r="P61" s="17"/>
+      <c r="O61" s="17"/>
+      <c r="P61" s="18"/>
     </row>
     <row r="62" spans="2:54" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="3">
         <v>131</v>
       </c>
-      <c r="C62" s="19">
+      <c r="C62" s="15">
         <v>8</v>
       </c>
       <c r="D62" s="3">
@@ -10600,7 +10600,7 @@
       <c r="F62" s="3">
         <v>141</v>
       </c>
-      <c r="G62" s="19">
+      <c r="G62" s="15">
         <v>16</v>
       </c>
       <c r="H62" s="3">
@@ -10609,7 +10609,7 @@
       <c r="J62" s="3">
         <v>133</v>
       </c>
-      <c r="K62" s="19">
+      <c r="K62" s="15">
         <v>5</v>
       </c>
       <c r="L62" s="3">
@@ -10618,7 +10618,7 @@
       <c r="N62" s="3">
         <v>136</v>
       </c>
-      <c r="O62" s="19">
+      <c r="O62" s="15">
         <v>6</v>
       </c>
       <c r="P62" s="3">
@@ -10669,32 +10669,32 @@
       </c>
     </row>
     <row r="65" spans="2:16" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="15">
+      <c r="B65" s="16">
         <v>6.4</v>
       </c>
-      <c r="C65" s="16"/>
-      <c r="D65" s="17"/>
-      <c r="F65" s="15">
+      <c r="C65" s="17"/>
+      <c r="D65" s="18"/>
+      <c r="F65" s="16">
         <v>6.5</v>
       </c>
-      <c r="G65" s="16"/>
-      <c r="H65" s="17"/>
-      <c r="J65" s="15">
+      <c r="G65" s="17"/>
+      <c r="H65" s="18"/>
+      <c r="J65" s="16">
         <v>6.6</v>
       </c>
-      <c r="K65" s="16"/>
-      <c r="L65" s="17"/>
-      <c r="N65" s="15">
+      <c r="K65" s="17"/>
+      <c r="L65" s="18"/>
+      <c r="N65" s="16">
         <v>6.7</v>
       </c>
-      <c r="O65" s="16"/>
-      <c r="P65" s="17"/>
+      <c r="O65" s="17"/>
+      <c r="P65" s="18"/>
     </row>
     <row r="66" spans="2:16" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="3">
         <v>135</v>
       </c>
-      <c r="C66" s="19">
+      <c r="C66" s="15">
         <v>2</v>
       </c>
       <c r="D66" s="3">
@@ -10703,7 +10703,7 @@
       <c r="F66" s="3">
         <v>137</v>
       </c>
-      <c r="G66" s="19">
+      <c r="G66" s="15">
         <v>0</v>
       </c>
       <c r="H66" s="3">
@@ -10712,7 +10712,7 @@
       <c r="J66" s="3">
         <v>139</v>
       </c>
-      <c r="K66" s="19">
+      <c r="K66" s="15">
         <v>0</v>
       </c>
       <c r="L66" s="3">
@@ -10721,7 +10721,7 @@
       <c r="N66" s="3">
         <v>142</v>
       </c>
-      <c r="O66" s="19">
+      <c r="O66" s="15">
         <v>0</v>
       </c>
       <c r="P66" s="3">
@@ -10730,14 +10730,54 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="J61:L61"/>
-    <mergeCell ref="N61:P61"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="J65:L65"/>
-    <mergeCell ref="N65:P65"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="J53:L53"/>
+    <mergeCell ref="N53:P53"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="J57:L57"/>
+    <mergeCell ref="N57:P57"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="J45:L45"/>
+    <mergeCell ref="N45:P45"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="J49:L49"/>
+    <mergeCell ref="N49:P49"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="N37:P37"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="N41:P41"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="N33:P33"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="N17:P17"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="N5:P5"/>
@@ -10747,54 +10787,14 @@
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="N33:P33"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="N37:P37"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="N41:P41"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="J45:L45"/>
-    <mergeCell ref="N45:P45"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="J49:L49"/>
-    <mergeCell ref="N49:P49"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="J53:L53"/>
-    <mergeCell ref="N53:P53"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="J57:L57"/>
-    <mergeCell ref="N57:P57"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="J61:L61"/>
+    <mergeCell ref="N61:P61"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="J65:L65"/>
+    <mergeCell ref="N65:P65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>